<commit_message>
Adding Final set of documents for Land Module
</commit_message>
<xml_diff>
--- a/master_data/SM_StowageFactor.xlsx
+++ b/master_data/SM_StowageFactor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MSCPJT\seaport-portal-MSQL\master_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B54F47AC-AC0B-4726-8E75-5902617FB6B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73C0532-64CE-4C6F-8A01-8AE2A91B1CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11100" yWindow="0" windowWidth="10065" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cargo_Ton_per_m2" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="103">
   <si>
     <t>Category</t>
   </si>
@@ -28,18 +28,6 @@
     <t>Cargo</t>
   </si>
   <si>
-    <t>Stowage Factor (m³/ton)</t>
-  </si>
-  <si>
-    <t>Density (ton/m³)</t>
-  </si>
-  <si>
-    <t>Stacking Height (m)</t>
-  </si>
-  <si>
-    <t>Tonnage per m² (ton/m²)</t>
-  </si>
-  <si>
     <t>Dry Bulk</t>
   </si>
   <si>
@@ -52,9 +40,6 @@
     <t>2.00 – 2.50</t>
   </si>
   <si>
-    <t>3.0</t>
-  </si>
-  <si>
     <t>6.0 – 7.5</t>
   </si>
   <si>
@@ -166,9 +151,6 @@
     <t>1.82 – 2.86</t>
   </si>
   <si>
-    <t>2.5</t>
-  </si>
-  <si>
     <t>4.5 – 7.1</t>
   </si>
   <si>
@@ -247,60 +229,122 @@
     <t>Container</t>
   </si>
   <si>
-    <t>Heavy Machinery / Steel</t>
-  </si>
-  <si>
-    <t>0.40 – 0.60</t>
-  </si>
-  <si>
-    <t>1.7 – 2.5</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>4.5 – 5.0</t>
-  </si>
-  <si>
-    <t>Cement Bags</t>
-  </si>
-  <si>
-    <t>3.0 – 4.0</t>
-  </si>
-  <si>
-    <t>Fertilizer Bags</t>
-  </si>
-  <si>
-    <t>2.5 – 3.0</t>
-  </si>
-  <si>
-    <t>Rice / Wheat</t>
-  </si>
-  <si>
     <t>1.30 – 1.60</t>
   </si>
   <si>
     <t>0.63 – 0.77</t>
   </si>
   <si>
-    <t>Cotton / Light Goods</t>
-  </si>
-  <si>
     <t>3.00 – 5.00</t>
   </si>
   <si>
     <t>0.20 – 0.33</t>
   </si>
   <si>
-    <t>0.5 – 1.0</t>
+    <t>20 Feet</t>
+  </si>
+  <si>
+    <t>40 Feet</t>
+  </si>
+  <si>
+    <t>45 Feet</t>
+  </si>
+  <si>
+    <t>60 Feet</t>
+  </si>
+  <si>
+    <t>StowageFactor</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>StowageFactorRagne</t>
+  </si>
+  <si>
+    <t>DensityRange</t>
+  </si>
+  <si>
+    <t>UOM</t>
+  </si>
+  <si>
+    <t>Cubic mts</t>
+  </si>
+  <si>
+    <t>SFUOM</t>
+  </si>
+  <si>
+    <t>SFRUOM</t>
+  </si>
+  <si>
+    <t>DRUOM</t>
+  </si>
+  <si>
+    <t>DUOM</t>
+  </si>
+  <si>
+    <t>14.8 -14.10</t>
+  </si>
+  <si>
+    <t>29.7 -30.0</t>
+  </si>
+  <si>
+    <t>33.4 -34.0</t>
+  </si>
+  <si>
+    <t>44.6 - 45.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StackingHeight </t>
+  </si>
+  <si>
+    <t>SHUOM</t>
+  </si>
+  <si>
+    <t>metre</t>
+  </si>
+  <si>
+    <t>TonnageRange</t>
+  </si>
+  <si>
+    <t>TRUOM</t>
+  </si>
+  <si>
+    <t>TON PER SQ MTS</t>
+  </si>
+  <si>
+    <t>Measure</t>
+  </si>
+  <si>
+    <t>20 ft</t>
+  </si>
+  <si>
+    <t>40 ft</t>
+  </si>
+  <si>
+    <t>45 ft</t>
+  </si>
+  <si>
+    <t>60 ft</t>
+  </si>
+  <si>
+    <t>tons</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -328,8 +372,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,12 +697,20 @@
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -656,437 +718,1074 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N1" t="s">
+        <v>95</v>
+      </c>
+      <c r="O1" t="s">
+        <v>97</v>
+      </c>
+      <c r="P1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2">
+        <v>0.5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="H2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2">
+        <v>2.5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K2" s="4">
+        <v>3</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="N2" t="s">
+        <v>96</v>
+      </c>
+      <c r="O2">
+        <v>7.5</v>
+      </c>
+      <c r="P2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3">
+        <v>1.5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3">
+        <v>0.77</v>
+      </c>
+      <c r="J3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="4">
+        <v>3</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="N3" t="s">
+        <v>96</v>
+      </c>
+      <c r="O3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="P3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I4">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="J4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K4" s="4">
+        <v>3</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="N4" t="s">
+        <v>96</v>
+      </c>
+      <c r="O4">
+        <v>3.33</v>
+      </c>
+      <c r="P4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5">
+        <v>0.83</v>
+      </c>
+      <c r="F5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5">
+        <v>1.59</v>
+      </c>
+      <c r="J5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5" s="4">
+        <v>3</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M5" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="N5" t="s">
+        <v>96</v>
+      </c>
+      <c r="O5">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="P5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="H6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I6">
+        <v>1.25</v>
+      </c>
+      <c r="J6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" s="4">
+        <v>3</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M6" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="N6" t="s">
+        <v>96</v>
+      </c>
+      <c r="O6">
+        <v>3.75</v>
+      </c>
+      <c r="P6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7">
+        <v>1.4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
+      <c r="H7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I7">
+        <v>0.77</v>
+      </c>
+      <c r="J7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" s="4">
+        <v>3</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M7" t="s">
         <v>26</v>
       </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="N7" t="s">
+        <v>96</v>
+      </c>
+      <c r="O7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="P7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8">
+        <v>1.6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
+      <c r="H8" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8">
+        <v>0.71</v>
+      </c>
+      <c r="J8" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="4">
+        <v>3</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M8" t="s">
         <v>30</v>
       </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="N8" t="s">
+        <v>96</v>
+      </c>
+      <c r="O8">
+        <v>2.1</v>
+      </c>
+      <c r="P8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9">
+        <v>1.4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" t="s">
         <v>33</v>
       </c>
-      <c r="D8" t="s">
+      <c r="H9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9">
+        <v>0.83</v>
+      </c>
+      <c r="J9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="4">
+        <v>3</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M9" t="s">
         <v>34</v>
       </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="N9" t="s">
+        <v>96</v>
+      </c>
+      <c r="O9">
+        <v>2.5</v>
+      </c>
+      <c r="P9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C10" t="s">
         <v>36</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10">
+        <v>1.2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="H10" t="s">
+        <v>82</v>
+      </c>
+      <c r="I10">
+        <v>0.91</v>
+      </c>
+      <c r="J10" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" s="4">
+        <v>3</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M10" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="N10" t="s">
+        <v>96</v>
+      </c>
+      <c r="O10">
+        <v>2.7</v>
+      </c>
+      <c r="P10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>41</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" t="s">
         <v>42</v>
       </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="H11" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11">
+        <v>2.86</v>
+      </c>
+      <c r="J11" t="s">
+        <v>82</v>
+      </c>
+      <c r="K11" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="N11" t="s">
+        <v>96</v>
+      </c>
+      <c r="O11">
+        <v>7.1</v>
+      </c>
+      <c r="P11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" t="s">
         <v>46</v>
       </c>
-      <c r="D11" t="s">
+      <c r="H12" t="s">
+        <v>82</v>
+      </c>
+      <c r="I12">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="J12" t="s">
+        <v>82</v>
+      </c>
+      <c r="K12" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M12" t="s">
         <v>47</v>
       </c>
-      <c r="E11" t="s">
+      <c r="N12" t="s">
+        <v>96</v>
+      </c>
+      <c r="O12">
+        <v>5.5</v>
+      </c>
+      <c r="P12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
         <v>48</v>
       </c>
-      <c r="F11" t="s">
+      <c r="C13" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13">
+        <v>1.4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" t="s">
         <v>50</v>
       </c>
-      <c r="C12" t="s">
+      <c r="H13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>82</v>
+      </c>
+      <c r="K13" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M13" t="s">
         <v>51</v>
       </c>
-      <c r="D12" t="s">
+      <c r="N13" t="s">
+        <v>96</v>
+      </c>
+      <c r="O13">
+        <v>2.5</v>
+      </c>
+      <c r="P13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
         <v>52</v>
       </c>
-      <c r="E12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="C14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14">
+        <v>1.35</v>
+      </c>
+      <c r="F14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" t="s">
         <v>54</v>
       </c>
-      <c r="C13" t="s">
+      <c r="H14" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14">
+        <v>0.83</v>
+      </c>
+      <c r="J14" t="s">
+        <v>82</v>
+      </c>
+      <c r="K14" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M14" t="s">
         <v>55</v>
       </c>
-      <c r="D13" t="s">
+      <c r="N14" t="s">
+        <v>96</v>
+      </c>
+      <c r="O14">
+        <v>2.08</v>
+      </c>
+      <c r="P14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
         <v>56</v>
       </c>
-      <c r="E13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="C15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" t="s">
         <v>58</v>
       </c>
-      <c r="C14" t="s">
+      <c r="H15" t="s">
+        <v>82</v>
+      </c>
+      <c r="I15">
+        <v>0.63</v>
+      </c>
+      <c r="J15" t="s">
+        <v>82</v>
+      </c>
+      <c r="K15" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M15" t="s">
         <v>59</v>
       </c>
-      <c r="D14" t="s">
+      <c r="N15" t="s">
+        <v>96</v>
+      </c>
+      <c r="O15">
+        <v>1.58</v>
+      </c>
+      <c r="P15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
         <v>60</v>
       </c>
-      <c r="E14" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="C16" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" t="s">
         <v>62</v>
       </c>
-      <c r="C15" t="s">
+      <c r="H16" t="s">
+        <v>82</v>
+      </c>
+      <c r="I16">
+        <v>0.83</v>
+      </c>
+      <c r="J16" t="s">
+        <v>82</v>
+      </c>
+      <c r="K16" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M16" t="s">
         <v>63</v>
       </c>
-      <c r="D15" t="s">
+      <c r="N16" t="s">
+        <v>96</v>
+      </c>
+      <c r="O16">
+        <v>2.08</v>
+      </c>
+      <c r="P16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
         <v>64</v>
       </c>
-      <c r="E15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="C17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="D17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" t="s">
         <v>66</v>
       </c>
-      <c r="C16" t="s">
+      <c r="H17" t="s">
+        <v>82</v>
+      </c>
+      <c r="I17">
+        <v>0.67</v>
+      </c>
+      <c r="J17" t="s">
+        <v>82</v>
+      </c>
+      <c r="K17" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M17" t="s">
         <v>67</v>
       </c>
-      <c r="D16" t="s">
+      <c r="N17" t="s">
+        <v>96</v>
+      </c>
+      <c r="O17">
+        <v>1.67</v>
+      </c>
+      <c r="P17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>68</v>
       </c>
-      <c r="E16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18">
+        <v>1.4</v>
+      </c>
+      <c r="F18" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>82</v>
+      </c>
+      <c r="K18">
+        <v>11.58</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M18" t="s">
+        <v>87</v>
+      </c>
+      <c r="N18" t="s">
+        <v>96</v>
+      </c>
+      <c r="O18">
+        <v>14.8</v>
+      </c>
+      <c r="P18" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19">
+        <v>1.35</v>
+      </c>
+      <c r="F19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" t="s">
+        <v>82</v>
+      </c>
+      <c r="I19">
+        <v>0.83</v>
+      </c>
+      <c r="J19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K19">
+        <v>11.58</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M19" t="s">
+        <v>88</v>
+      </c>
+      <c r="N19" t="s">
+        <v>96</v>
+      </c>
+      <c r="O19">
+        <v>29.7</v>
+      </c>
+      <c r="P19" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="3"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="D20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20">
+        <v>1.6</v>
+      </c>
+      <c r="F20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" t="s">
         <v>70</v>
       </c>
-      <c r="C17" t="s">
+      <c r="H20" t="s">
+        <v>82</v>
+      </c>
+      <c r="I20">
+        <v>0.77</v>
+      </c>
+      <c r="J20" t="s">
+        <v>82</v>
+      </c>
+      <c r="K20">
+        <v>11.58</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M20" t="s">
+        <v>89</v>
+      </c>
+      <c r="N20" t="s">
+        <v>96</v>
+      </c>
+      <c r="O20">
+        <v>33.4</v>
+      </c>
+      <c r="P20" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="3"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" t="s">
         <v>71</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21" t="s">
         <v>72</v>
       </c>
-      <c r="E17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" t="s">
-        <v>78</v>
-      </c>
-      <c r="F18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" t="s">
-        <v>89</v>
-      </c>
-      <c r="E22" t="s">
-        <v>78</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="H21" t="s">
+        <v>82</v>
+      </c>
+      <c r="I21">
+        <v>0.33</v>
+      </c>
+      <c r="J21" t="s">
+        <v>82</v>
+      </c>
+      <c r="K21">
+        <v>11.58</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M21" t="s">
         <v>90</v>
       </c>
+      <c r="N21" t="s">
+        <v>96</v>
+      </c>
+      <c r="O21">
+        <v>44.6</v>
+      </c>
+      <c r="P21" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="3"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>